<commit_message>
Scripts BDD et autres
</commit_message>
<xml_diff>
--- a/Documentations/planification-micdesgalier.xlsx
+++ b/Documentations/planification-micdesgalier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NeyzaX\Desktop\LAJA\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE081199-98C3-44E9-905F-A7622D960026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00393187-48B5-439B-885F-7B4DE903BA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3035D901-BB22-48CF-B0C5-43B325BB06A4}"/>
   </bookViews>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B68F59-51BD-4CD4-BB6D-8338FE525268}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>